<commit_message>
Add datasets 30-49 and update index
</commit_message>
<xml_diff>
--- a/Index.xlsx
+++ b/Index.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mkrangle\Documents\Projects\PACT\PACT Submissions\Range Angle Structured\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{C278D388-98ED-4A39-A3BA-19214D36E6E0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A89CEEB-F1CD-4F91-82B8-D85AE6FACDBF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28635" yWindow="-615" windowWidth="28020" windowHeight="14565"/>
+    <workbookView xWindow="-27120" yWindow="-555" windowWidth="26040" windowHeight="13920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index_structured" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="651" uniqueCount="116">
   <si>
     <t>environment_1</t>
   </si>
@@ -284,12 +284,99 @@
   </si>
   <si>
     <t>partner_beacon_id</t>
+  </si>
+  <si>
+    <t>set_30</t>
+  </si>
+  <si>
+    <t>hallway</t>
+  </si>
+  <si>
+    <t>motorola</t>
+  </si>
+  <si>
+    <t>set_31</t>
+  </si>
+  <si>
+    <t>set_32</t>
+  </si>
+  <si>
+    <t>Galaxy S9+</t>
+  </si>
+  <si>
+    <t>set_33</t>
+  </si>
+  <si>
+    <t>Pixel 4</t>
+  </si>
+  <si>
+    <t>set_34</t>
+  </si>
+  <si>
+    <t>set_35</t>
+  </si>
+  <si>
+    <t>structured_Test Protocol Mid</t>
+  </si>
+  <si>
+    <t>set_36</t>
+  </si>
+  <si>
+    <t>Moto x4</t>
+  </si>
+  <si>
+    <t>set_37</t>
+  </si>
+  <si>
+    <t>set_38</t>
+  </si>
+  <si>
+    <t>set_39</t>
+  </si>
+  <si>
+    <t>set_40</t>
+  </si>
+  <si>
+    <t>set_41</t>
+  </si>
+  <si>
+    <t>pixel2</t>
+  </si>
+  <si>
+    <t>set_42</t>
+  </si>
+  <si>
+    <t>set_43</t>
+  </si>
+  <si>
+    <t>iPhone 5s</t>
+  </si>
+  <si>
+    <t>set_44</t>
+  </si>
+  <si>
+    <t>set_45</t>
+  </si>
+  <si>
+    <t>moto g7</t>
+  </si>
+  <si>
+    <t>set_46</t>
+  </si>
+  <si>
+    <t>set_47</t>
+  </si>
+  <si>
+    <t>set_48</t>
+  </si>
+  <si>
+    <t>set_49</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1140,11 +1227,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N30"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:N50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1:N1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="K31" sqref="K31:K50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2482,8 +2569,888 @@
         <v>13</v>
       </c>
     </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>87</v>
+      </c>
+      <c r="B31" t="s">
+        <v>3</v>
+      </c>
+      <c r="C31" t="s">
+        <v>4</v>
+      </c>
+      <c r="D31" t="s">
+        <v>20</v>
+      </c>
+      <c r="E31">
+        <v>8</v>
+      </c>
+      <c r="F31" t="s">
+        <v>88</v>
+      </c>
+      <c r="G31" t="s">
+        <v>44</v>
+      </c>
+      <c r="H31" t="s">
+        <v>23</v>
+      </c>
+      <c r="I31" t="s">
+        <v>9</v>
+      </c>
+      <c r="J31" t="s">
+        <v>8</v>
+      </c>
+      <c r="K31" t="s">
+        <v>89</v>
+      </c>
+      <c r="L31" t="s">
+        <v>9</v>
+      </c>
+      <c r="M31" t="s">
+        <v>8</v>
+      </c>
+      <c r="N31" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>90</v>
+      </c>
+      <c r="B32" t="s">
+        <v>3</v>
+      </c>
+      <c r="C32" t="s">
+        <v>4</v>
+      </c>
+      <c r="D32" t="s">
+        <v>20</v>
+      </c>
+      <c r="E32">
+        <v>8</v>
+      </c>
+      <c r="F32" t="s">
+        <v>14</v>
+      </c>
+      <c r="G32" t="s">
+        <v>21</v>
+      </c>
+      <c r="H32" t="s">
+        <v>17</v>
+      </c>
+      <c r="I32" t="s">
+        <v>9</v>
+      </c>
+      <c r="J32" t="s">
+        <v>8</v>
+      </c>
+      <c r="K32" t="s">
+        <v>16</v>
+      </c>
+      <c r="L32" t="s">
+        <v>9</v>
+      </c>
+      <c r="M32" t="s">
+        <v>8</v>
+      </c>
+      <c r="N32" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>91</v>
+      </c>
+      <c r="B33" t="s">
+        <v>3</v>
+      </c>
+      <c r="C33" t="s">
+        <v>4</v>
+      </c>
+      <c r="D33" t="s">
+        <v>20</v>
+      </c>
+      <c r="E33">
+        <v>8</v>
+      </c>
+      <c r="F33" t="s">
+        <v>6</v>
+      </c>
+      <c r="G33" t="s">
+        <v>44</v>
+      </c>
+      <c r="H33" t="s">
+        <v>23</v>
+      </c>
+      <c r="I33" t="s">
+        <v>15</v>
+      </c>
+      <c r="J33" t="s">
+        <v>27</v>
+      </c>
+      <c r="K33" t="s">
+        <v>92</v>
+      </c>
+      <c r="L33" t="s">
+        <v>9</v>
+      </c>
+      <c r="M33" t="s">
+        <v>8</v>
+      </c>
+      <c r="N33" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>93</v>
+      </c>
+      <c r="B34" t="s">
+        <v>3</v>
+      </c>
+      <c r="C34" t="s">
+        <v>4</v>
+      </c>
+      <c r="D34" t="s">
+        <v>20</v>
+      </c>
+      <c r="E34">
+        <v>8</v>
+      </c>
+      <c r="F34" t="s">
+        <v>88</v>
+      </c>
+      <c r="G34" t="s">
+        <v>7</v>
+      </c>
+      <c r="H34" t="s">
+        <v>17</v>
+      </c>
+      <c r="I34" t="s">
+        <v>9</v>
+      </c>
+      <c r="J34" t="s">
+        <v>8</v>
+      </c>
+      <c r="K34" t="s">
+        <v>94</v>
+      </c>
+      <c r="L34" t="s">
+        <v>15</v>
+      </c>
+      <c r="M34" t="s">
+        <v>8</v>
+      </c>
+      <c r="N34" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>95</v>
+      </c>
+      <c r="B35" t="s">
+        <v>3</v>
+      </c>
+      <c r="C35" t="s">
+        <v>4</v>
+      </c>
+      <c r="D35" t="s">
+        <v>20</v>
+      </c>
+      <c r="E35">
+        <v>8</v>
+      </c>
+      <c r="F35" t="s">
+        <v>54</v>
+      </c>
+      <c r="G35" t="s">
+        <v>21</v>
+      </c>
+      <c r="H35" t="s">
+        <v>23</v>
+      </c>
+      <c r="I35" t="s">
+        <v>9</v>
+      </c>
+      <c r="J35" t="s">
+        <v>8</v>
+      </c>
+      <c r="K35" t="s">
+        <v>22</v>
+      </c>
+      <c r="L35" t="s">
+        <v>15</v>
+      </c>
+      <c r="M35" t="s">
+        <v>8</v>
+      </c>
+      <c r="N35" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>96</v>
+      </c>
+      <c r="B36" t="s">
+        <v>3</v>
+      </c>
+      <c r="C36" t="s">
+        <v>4</v>
+      </c>
+      <c r="D36" t="s">
+        <v>97</v>
+      </c>
+      <c r="E36">
+        <v>5</v>
+      </c>
+      <c r="F36" t="s">
+        <v>54</v>
+      </c>
+      <c r="G36" t="s">
+        <v>7</v>
+      </c>
+      <c r="H36" t="s">
+        <v>17</v>
+      </c>
+      <c r="I36" t="s">
+        <v>15</v>
+      </c>
+      <c r="J36" t="s">
+        <v>8</v>
+      </c>
+      <c r="K36" t="s">
+        <v>39</v>
+      </c>
+      <c r="L36" t="s">
+        <v>15</v>
+      </c>
+      <c r="M36" t="s">
+        <v>8</v>
+      </c>
+      <c r="N36" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>98</v>
+      </c>
+      <c r="B37" t="s">
+        <v>3</v>
+      </c>
+      <c r="C37" t="s">
+        <v>4</v>
+      </c>
+      <c r="D37" t="s">
+        <v>20</v>
+      </c>
+      <c r="E37">
+        <v>8</v>
+      </c>
+      <c r="F37" t="s">
+        <v>54</v>
+      </c>
+      <c r="G37" t="s">
+        <v>7</v>
+      </c>
+      <c r="H37" t="s">
+        <v>11</v>
+      </c>
+      <c r="I37" t="s">
+        <v>9</v>
+      </c>
+      <c r="J37" t="s">
+        <v>27</v>
+      </c>
+      <c r="K37" t="s">
+        <v>99</v>
+      </c>
+      <c r="L37" t="s">
+        <v>9</v>
+      </c>
+      <c r="M37" t="s">
+        <v>27</v>
+      </c>
+      <c r="N37" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>100</v>
+      </c>
+      <c r="B38" t="s">
+        <v>3</v>
+      </c>
+      <c r="C38" t="s">
+        <v>4</v>
+      </c>
+      <c r="D38" t="s">
+        <v>20</v>
+      </c>
+      <c r="E38">
+        <v>8</v>
+      </c>
+      <c r="F38" t="s">
+        <v>54</v>
+      </c>
+      <c r="G38" t="s">
+        <v>44</v>
+      </c>
+      <c r="H38" t="s">
+        <v>17</v>
+      </c>
+      <c r="I38" t="s">
+        <v>9</v>
+      </c>
+      <c r="J38" t="s">
+        <v>8</v>
+      </c>
+      <c r="K38" t="s">
+        <v>26</v>
+      </c>
+      <c r="L38" t="s">
+        <v>15</v>
+      </c>
+      <c r="M38" t="s">
+        <v>27</v>
+      </c>
+      <c r="N38" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>101</v>
+      </c>
+      <c r="B39" t="s">
+        <v>3</v>
+      </c>
+      <c r="C39" t="s">
+        <v>4</v>
+      </c>
+      <c r="D39" t="s">
+        <v>20</v>
+      </c>
+      <c r="E39">
+        <v>9</v>
+      </c>
+      <c r="F39" t="s">
+        <v>54</v>
+      </c>
+      <c r="G39" t="s">
+        <v>7</v>
+      </c>
+      <c r="H39" t="s">
+        <v>61</v>
+      </c>
+      <c r="I39" t="s">
+        <v>9</v>
+      </c>
+      <c r="J39" t="s">
+        <v>25</v>
+      </c>
+      <c r="K39" t="s">
+        <v>35</v>
+      </c>
+      <c r="L39" t="s">
+        <v>15</v>
+      </c>
+      <c r="M39" t="s">
+        <v>38</v>
+      </c>
+      <c r="N39" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>102</v>
+      </c>
+      <c r="B40" t="s">
+        <v>3</v>
+      </c>
+      <c r="C40" t="s">
+        <v>4</v>
+      </c>
+      <c r="D40" t="s">
+        <v>20</v>
+      </c>
+      <c r="E40">
+        <v>8</v>
+      </c>
+      <c r="F40" t="s">
+        <v>54</v>
+      </c>
+      <c r="G40" t="s">
+        <v>44</v>
+      </c>
+      <c r="H40" t="s">
+        <v>49</v>
+      </c>
+      <c r="I40" t="s">
+        <v>9</v>
+      </c>
+      <c r="J40" t="s">
+        <v>8</v>
+      </c>
+      <c r="K40" t="s">
+        <v>10</v>
+      </c>
+      <c r="L40" t="s">
+        <v>9</v>
+      </c>
+      <c r="M40" t="s">
+        <v>27</v>
+      </c>
+      <c r="N40" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>103</v>
+      </c>
+      <c r="B41" t="s">
+        <v>3</v>
+      </c>
+      <c r="C41" t="s">
+        <v>4</v>
+      </c>
+      <c r="D41" t="s">
+        <v>20</v>
+      </c>
+      <c r="E41">
+        <v>8</v>
+      </c>
+      <c r="F41" t="s">
+        <v>14</v>
+      </c>
+      <c r="G41" t="s">
+        <v>44</v>
+      </c>
+      <c r="H41" t="s">
+        <v>17</v>
+      </c>
+      <c r="I41" t="s">
+        <v>15</v>
+      </c>
+      <c r="J41" t="s">
+        <v>8</v>
+      </c>
+      <c r="K41" t="s">
+        <v>39</v>
+      </c>
+      <c r="L41" t="s">
+        <v>15</v>
+      </c>
+      <c r="M41" t="s">
+        <v>8</v>
+      </c>
+      <c r="N41" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>104</v>
+      </c>
+      <c r="B42" t="s">
+        <v>3</v>
+      </c>
+      <c r="C42" t="s">
+        <v>4</v>
+      </c>
+      <c r="D42" t="s">
+        <v>20</v>
+      </c>
+      <c r="E42">
+        <v>8</v>
+      </c>
+      <c r="F42" t="s">
+        <v>6</v>
+      </c>
+      <c r="G42" t="s">
+        <v>21</v>
+      </c>
+      <c r="H42" t="s">
+        <v>17</v>
+      </c>
+      <c r="I42" t="s">
+        <v>9</v>
+      </c>
+      <c r="J42" t="s">
+        <v>8</v>
+      </c>
+      <c r="K42" t="s">
+        <v>105</v>
+      </c>
+      <c r="L42" t="s">
+        <v>9</v>
+      </c>
+      <c r="M42" t="s">
+        <v>8</v>
+      </c>
+      <c r="N42" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>106</v>
+      </c>
+      <c r="B43" t="s">
+        <v>3</v>
+      </c>
+      <c r="C43" t="s">
+        <v>4</v>
+      </c>
+      <c r="D43" t="s">
+        <v>20</v>
+      </c>
+      <c r="E43">
+        <v>5</v>
+      </c>
+      <c r="F43" t="s">
+        <v>6</v>
+      </c>
+      <c r="G43" t="s">
+        <v>21</v>
+      </c>
+      <c r="H43" t="s">
+        <v>17</v>
+      </c>
+      <c r="I43" t="s">
+        <v>15</v>
+      </c>
+      <c r="J43" t="s">
+        <v>27</v>
+      </c>
+      <c r="K43" t="s">
+        <v>105</v>
+      </c>
+      <c r="L43" t="s">
+        <v>15</v>
+      </c>
+      <c r="M43" t="s">
+        <v>38</v>
+      </c>
+      <c r="N43" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>107</v>
+      </c>
+      <c r="B44" t="s">
+        <v>3</v>
+      </c>
+      <c r="C44" t="s">
+        <v>4</v>
+      </c>
+      <c r="D44" t="s">
+        <v>20</v>
+      </c>
+      <c r="E44">
+        <v>8</v>
+      </c>
+      <c r="F44" t="s">
+        <v>88</v>
+      </c>
+      <c r="G44" t="s">
+        <v>44</v>
+      </c>
+      <c r="H44" t="s">
+        <v>23</v>
+      </c>
+      <c r="I44" t="s">
+        <v>9</v>
+      </c>
+      <c r="J44" t="s">
+        <v>27</v>
+      </c>
+      <c r="K44" t="s">
+        <v>108</v>
+      </c>
+      <c r="L44" t="s">
+        <v>9</v>
+      </c>
+      <c r="M44" t="s">
+        <v>8</v>
+      </c>
+      <c r="N44" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>109</v>
+      </c>
+      <c r="B45" t="s">
+        <v>3</v>
+      </c>
+      <c r="C45" t="s">
+        <v>4</v>
+      </c>
+      <c r="D45" t="s">
+        <v>20</v>
+      </c>
+      <c r="E45">
+        <v>8</v>
+      </c>
+      <c r="F45" t="s">
+        <v>88</v>
+      </c>
+      <c r="G45" t="s">
+        <v>7</v>
+      </c>
+      <c r="H45" t="s">
+        <v>23</v>
+      </c>
+      <c r="I45" t="s">
+        <v>9</v>
+      </c>
+      <c r="J45" t="s">
+        <v>8</v>
+      </c>
+      <c r="K45" t="s">
+        <v>57</v>
+      </c>
+      <c r="L45" t="s">
+        <v>15</v>
+      </c>
+      <c r="M45" t="s">
+        <v>8</v>
+      </c>
+      <c r="N45" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>110</v>
+      </c>
+      <c r="B46" t="s">
+        <v>3</v>
+      </c>
+      <c r="C46" t="s">
+        <v>4</v>
+      </c>
+      <c r="D46" t="s">
+        <v>20</v>
+      </c>
+      <c r="E46">
+        <v>8</v>
+      </c>
+      <c r="F46" t="s">
+        <v>14</v>
+      </c>
+      <c r="G46" t="s">
+        <v>21</v>
+      </c>
+      <c r="H46" t="s">
+        <v>17</v>
+      </c>
+      <c r="I46" t="s">
+        <v>9</v>
+      </c>
+      <c r="J46" t="s">
+        <v>8</v>
+      </c>
+      <c r="K46" t="s">
+        <v>111</v>
+      </c>
+      <c r="L46" t="s">
+        <v>9</v>
+      </c>
+      <c r="M46" t="s">
+        <v>8</v>
+      </c>
+      <c r="N46" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>112</v>
+      </c>
+      <c r="B47" t="s">
+        <v>3</v>
+      </c>
+      <c r="C47" t="s">
+        <v>4</v>
+      </c>
+      <c r="D47" t="s">
+        <v>20</v>
+      </c>
+      <c r="E47">
+        <v>8</v>
+      </c>
+      <c r="F47" t="s">
+        <v>29</v>
+      </c>
+      <c r="G47" t="s">
+        <v>7</v>
+      </c>
+      <c r="H47" t="s">
+        <v>11</v>
+      </c>
+      <c r="I47" t="s">
+        <v>9</v>
+      </c>
+      <c r="J47" t="s">
+        <v>8</v>
+      </c>
+      <c r="K47" t="s">
+        <v>39</v>
+      </c>
+      <c r="L47" t="s">
+        <v>9</v>
+      </c>
+      <c r="M47" t="s">
+        <v>8</v>
+      </c>
+      <c r="N47" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>113</v>
+      </c>
+      <c r="B48" t="s">
+        <v>3</v>
+      </c>
+      <c r="C48" t="s">
+        <v>4</v>
+      </c>
+      <c r="D48" t="s">
+        <v>97</v>
+      </c>
+      <c r="E48">
+        <v>5</v>
+      </c>
+      <c r="F48" t="s">
+        <v>14</v>
+      </c>
+      <c r="G48" t="s">
+        <v>7</v>
+      </c>
+      <c r="H48" t="s">
+        <v>49</v>
+      </c>
+      <c r="I48" t="s">
+        <v>15</v>
+      </c>
+      <c r="J48" t="s">
+        <v>8</v>
+      </c>
+      <c r="K48" t="s">
+        <v>10</v>
+      </c>
+      <c r="L48" t="s">
+        <v>9</v>
+      </c>
+      <c r="M48" t="s">
+        <v>8</v>
+      </c>
+      <c r="N48" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>114</v>
+      </c>
+      <c r="B49" t="s">
+        <v>3</v>
+      </c>
+      <c r="C49" t="s">
+        <v>4</v>
+      </c>
+      <c r="D49" t="s">
+        <v>97</v>
+      </c>
+      <c r="E49">
+        <v>5</v>
+      </c>
+      <c r="F49" t="s">
+        <v>14</v>
+      </c>
+      <c r="G49" t="s">
+        <v>44</v>
+      </c>
+      <c r="H49" t="s">
+        <v>17</v>
+      </c>
+      <c r="I49" t="s">
+        <v>9</v>
+      </c>
+      <c r="J49" t="s">
+        <v>8</v>
+      </c>
+      <c r="K49" t="s">
+        <v>39</v>
+      </c>
+      <c r="L49" t="s">
+        <v>9</v>
+      </c>
+      <c r="M49" t="s">
+        <v>38</v>
+      </c>
+      <c r="N49" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>115</v>
+      </c>
+      <c r="B50" t="s">
+        <v>3</v>
+      </c>
+      <c r="C50" t="s">
+        <v>4</v>
+      </c>
+      <c r="D50" t="s">
+        <v>20</v>
+      </c>
+      <c r="E50">
+        <v>8</v>
+      </c>
+      <c r="F50" t="s">
+        <v>54</v>
+      </c>
+      <c r="G50" t="s">
+        <v>7</v>
+      </c>
+      <c r="H50" t="s">
+        <v>31</v>
+      </c>
+      <c r="I50" t="s">
+        <v>9</v>
+      </c>
+      <c r="J50" t="s">
+        <v>8</v>
+      </c>
+      <c r="K50" t="s">
+        <v>65</v>
+      </c>
+      <c r="L50" t="s">
+        <v>15</v>
+      </c>
+      <c r="M50" t="s">
+        <v>8</v>
+      </c>
+      <c r="N50" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:Q30"/>
+  <autoFilter ref="A1:Q30" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Y32">
     <sortCondition ref="A2:A32"/>
   </sortState>

</xml_diff>

<commit_message>
Add sets 72-74, delete sets 43, 53, 56 and 57
</commit_message>
<xml_diff>
--- a/Index.xlsx
+++ b/Index.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mkrangle\Documents\Projects\PACT\PACT Submissions\Range Angle Structured\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B29FF584-8256-4057-A62A-BFA087A0FD67}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F719CB73-F18D-46D9-AE4D-CE8FDC86A705}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="8130" windowWidth="27345" windowHeight="9705" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2130" yWindow="2505" windowWidth="27285" windowHeight="14010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index_structured" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="937" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="924" uniqueCount="146">
   <si>
     <t>environment_1</t>
   </si>
@@ -343,9 +343,6 @@
     <t>pixel2</t>
   </si>
   <si>
-    <t>set_42</t>
-  </si>
-  <si>
     <t>set_43</t>
   </si>
   <si>
@@ -388,9 +385,6 @@
     <t>set_52</t>
   </si>
   <si>
-    <t>set_53</t>
-  </si>
-  <si>
     <t>set_54</t>
   </si>
   <si>
@@ -403,12 +397,6 @@
     <t>iPhone 6 Plus</t>
   </si>
   <si>
-    <t>set_56</t>
-  </si>
-  <si>
-    <t>set_57</t>
-  </si>
-  <si>
     <t>set_58</t>
   </si>
   <si>
@@ -458,6 +446,21 @@
   </si>
   <si>
     <t xml:space="preserve"> iPhone X</t>
+  </si>
+  <si>
+    <t>set_72</t>
+  </si>
+  <si>
+    <t>Google Pixel 2</t>
+  </si>
+  <si>
+    <t>set_73</t>
+  </si>
+  <si>
+    <t>Samsung Galaxy S10</t>
+  </si>
+  <si>
+    <t>set_74</t>
   </si>
 </sst>
 </file>
@@ -1315,28 +1318,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N72"/>
+  <dimension ref="A1:N71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="A65" sqref="A65:N72"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="A72" sqref="A72:XFD72"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="11.42578125" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" customWidth="1"/>
-    <col min="4" max="4" width="28.5703125" customWidth="1"/>
-    <col min="6" max="6" width="15.42578125" customWidth="1"/>
-    <col min="7" max="7" width="20.5703125" customWidth="1"/>
-    <col min="8" max="9" width="15.42578125" customWidth="1"/>
-    <col min="10" max="10" width="20.5703125" customWidth="1"/>
-    <col min="11" max="11" width="19.140625" customWidth="1"/>
-    <col min="12" max="12" width="15.42578125" customWidth="1"/>
-    <col min="13" max="13" width="20.5703125" customWidth="1"/>
-    <col min="14" max="14" width="15.42578125" customWidth="1"/>
+    <col min="2" max="2" width="11.453125" customWidth="1"/>
+    <col min="3" max="3" width="13.453125" customWidth="1"/>
+    <col min="4" max="4" width="28.54296875" customWidth="1"/>
+    <col min="6" max="6" width="15.453125" customWidth="1"/>
+    <col min="7" max="7" width="20.54296875" customWidth="1"/>
+    <col min="8" max="9" width="15.453125" customWidth="1"/>
+    <col min="10" max="10" width="20.54296875" customWidth="1"/>
+    <col min="11" max="11" width="19.1796875" customWidth="1"/>
+    <col min="12" max="12" width="15.453125" customWidth="1"/>
+    <col min="13" max="13" width="20.54296875" customWidth="1"/>
+    <col min="14" max="14" width="15.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -1380,7 +1383,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>24</v>
       </c>
@@ -1424,7 +1427,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>69</v>
       </c>
@@ -1468,7 +1471,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>48</v>
       </c>
@@ -1512,7 +1515,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>67</v>
       </c>
@@ -1556,7 +1559,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>28</v>
       </c>
@@ -1600,7 +1603,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>32</v>
       </c>
@@ -1644,7 +1647,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>59</v>
       </c>
@@ -1688,7 +1691,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>64</v>
       </c>
@@ -1732,7 +1735,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>50</v>
       </c>
@@ -1776,7 +1779,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>62</v>
       </c>
@@ -1820,7 +1823,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>73</v>
       </c>
@@ -1864,7 +1867,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>36</v>
       </c>
@@ -1908,7 +1911,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>52</v>
       </c>
@@ -1952,7 +1955,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>40</v>
       </c>
@@ -1996,7 +1999,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -2040,7 +2043,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>34</v>
       </c>
@@ -2084,7 +2087,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>47</v>
       </c>
@@ -2128,7 +2131,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>71</v>
       </c>
@@ -2172,7 +2175,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>60</v>
       </c>
@@ -2216,7 +2219,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>56</v>
       </c>
@@ -2260,7 +2263,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>75</v>
       </c>
@@ -2304,7 +2307,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>72</v>
       </c>
@@ -2348,7 +2351,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>63</v>
       </c>
@@ -2392,7 +2395,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>58</v>
       </c>
@@ -2436,7 +2439,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>12</v>
       </c>
@@ -2480,7 +2483,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>66</v>
       </c>
@@ -2524,7 +2527,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>53</v>
       </c>
@@ -2568,7 +2571,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>43</v>
       </c>
@@ -2612,7 +2615,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>46</v>
       </c>
@@ -2656,7 +2659,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>87</v>
       </c>
@@ -2700,7 +2703,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>90</v>
       </c>
@@ -2744,7 +2747,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>91</v>
       </c>
@@ -2788,7 +2791,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>93</v>
       </c>
@@ -2832,7 +2835,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>95</v>
       </c>
@@ -2876,7 +2879,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>96</v>
       </c>
@@ -2920,7 +2923,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>98</v>
       </c>
@@ -2964,7 +2967,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>100</v>
       </c>
@@ -3008,7 +3011,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>101</v>
       </c>
@@ -3052,7 +3055,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>102</v>
       </c>
@@ -3096,7 +3099,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>103</v>
       </c>
@@ -3140,7 +3143,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>104</v>
       </c>
@@ -3184,7 +3187,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>106</v>
       </c>
@@ -3198,39 +3201,39 @@
         <v>20</v>
       </c>
       <c r="E43">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F43" t="s">
-        <v>6</v>
+        <v>88</v>
       </c>
       <c r="G43" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="H43" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="I43" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="J43" t="s">
         <v>27</v>
       </c>
       <c r="K43" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="L43" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="M43" t="s">
-        <v>38</v>
+        <v>8</v>
       </c>
       <c r="N43" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B44" t="s">
         <v>3</v>
@@ -3248,7 +3251,7 @@
         <v>88</v>
       </c>
       <c r="G44" t="s">
-        <v>44</v>
+        <v>7</v>
       </c>
       <c r="H44" t="s">
         <v>23</v>
@@ -3257,13 +3260,13 @@
         <v>9</v>
       </c>
       <c r="J44" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="K44" t="s">
-        <v>108</v>
+        <v>57</v>
       </c>
       <c r="L44" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="M44" t="s">
         <v>8</v>
@@ -3272,7 +3275,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>109</v>
       </c>
@@ -3289,13 +3292,13 @@
         <v>8</v>
       </c>
       <c r="F45" t="s">
-        <v>88</v>
+        <v>14</v>
       </c>
       <c r="G45" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="H45" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="I45" t="s">
         <v>9</v>
@@ -3304,10 +3307,10 @@
         <v>8</v>
       </c>
       <c r="K45" t="s">
-        <v>57</v>
+        <v>110</v>
       </c>
       <c r="L45" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="M45" t="s">
         <v>8</v>
@@ -3316,9 +3319,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B46" t="s">
         <v>3</v>
@@ -3333,13 +3336,13 @@
         <v>8</v>
       </c>
       <c r="F46" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="G46" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="H46" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="I46" t="s">
         <v>9</v>
@@ -3348,7 +3351,7 @@
         <v>8</v>
       </c>
       <c r="K46" t="s">
-        <v>111</v>
+        <v>39</v>
       </c>
       <c r="L46" t="s">
         <v>9</v>
@@ -3360,7 +3363,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>112</v>
       </c>
@@ -3371,28 +3374,28 @@
         <v>4</v>
       </c>
       <c r="D47" t="s">
-        <v>20</v>
+        <v>97</v>
       </c>
       <c r="E47">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F47" t="s">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="G47" t="s">
         <v>7</v>
       </c>
       <c r="H47" t="s">
-        <v>11</v>
+        <v>49</v>
       </c>
       <c r="I47" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="J47" t="s">
         <v>8</v>
       </c>
       <c r="K47" t="s">
-        <v>39</v>
+        <v>10</v>
       </c>
       <c r="L47" t="s">
         <v>9</v>
@@ -3404,7 +3407,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>113</v>
       </c>
@@ -3424,31 +3427,31 @@
         <v>14</v>
       </c>
       <c r="G48" t="s">
-        <v>7</v>
+        <v>44</v>
       </c>
       <c r="H48" t="s">
-        <v>49</v>
+        <v>17</v>
       </c>
       <c r="I48" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="J48" t="s">
         <v>8</v>
       </c>
       <c r="K48" t="s">
-        <v>10</v>
+        <v>39</v>
       </c>
       <c r="L48" t="s">
         <v>9</v>
       </c>
       <c r="M48" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="N48" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>114</v>
       </c>
@@ -3459,19 +3462,19 @@
         <v>4</v>
       </c>
       <c r="D49" t="s">
-        <v>97</v>
+        <v>20</v>
       </c>
       <c r="E49">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F49" t="s">
-        <v>14</v>
+        <v>54</v>
       </c>
       <c r="G49" t="s">
-        <v>44</v>
+        <v>7</v>
       </c>
       <c r="H49" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="I49" t="s">
         <v>9</v>
@@ -3480,63 +3483,63 @@
         <v>8</v>
       </c>
       <c r="K49" t="s">
-        <v>39</v>
+        <v>65</v>
       </c>
       <c r="L49" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="M49" t="s">
-        <v>38</v>
+        <v>8</v>
       </c>
       <c r="N49" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
+        <v>116</v>
+      </c>
+      <c r="B50" t="s">
+        <v>3</v>
+      </c>
+      <c r="C50" t="s">
+        <v>4</v>
+      </c>
+      <c r="D50" t="s">
+        <v>20</v>
+      </c>
+      <c r="E50">
+        <v>8</v>
+      </c>
+      <c r="F50" t="s">
+        <v>6</v>
+      </c>
+      <c r="G50" t="s">
+        <v>7</v>
+      </c>
+      <c r="H50" t="s">
+        <v>11</v>
+      </c>
+      <c r="I50" t="s">
+        <v>9</v>
+      </c>
+      <c r="J50" t="s">
+        <v>27</v>
+      </c>
+      <c r="K50" t="s">
         <v>115</v>
       </c>
-      <c r="B50" t="s">
-        <v>3</v>
-      </c>
-      <c r="C50" t="s">
-        <v>4</v>
-      </c>
-      <c r="D50" t="s">
-        <v>20</v>
-      </c>
-      <c r="E50">
-        <v>8</v>
-      </c>
-      <c r="F50" t="s">
-        <v>54</v>
-      </c>
-      <c r="G50" t="s">
-        <v>7</v>
-      </c>
-      <c r="H50" t="s">
-        <v>31</v>
-      </c>
-      <c r="I50" t="s">
-        <v>9</v>
-      </c>
-      <c r="J50" t="s">
-        <v>8</v>
-      </c>
-      <c r="K50" t="s">
-        <v>65</v>
-      </c>
       <c r="L50" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="M50" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="N50" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>117</v>
       </c>
@@ -3556,33 +3559,33 @@
         <v>6</v>
       </c>
       <c r="G51" t="s">
-        <v>7</v>
+        <v>37</v>
       </c>
       <c r="H51" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="I51" t="s">
         <v>9</v>
       </c>
       <c r="J51" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="K51" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="L51" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="M51" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="N51" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B52" t="s">
         <v>3</v>
@@ -3597,25 +3600,25 @@
         <v>8</v>
       </c>
       <c r="F52" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="G52" t="s">
-        <v>37</v>
+        <v>7</v>
       </c>
       <c r="H52" t="s">
-        <v>23</v>
+        <v>49</v>
       </c>
       <c r="I52" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="J52" t="s">
         <v>8</v>
       </c>
       <c r="K52" t="s">
-        <v>119</v>
+        <v>35</v>
       </c>
       <c r="L52" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="M52" t="s">
         <v>8</v>
@@ -3624,7 +3627,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>120</v>
       </c>
@@ -3641,36 +3644,36 @@
         <v>8</v>
       </c>
       <c r="F53" t="s">
-        <v>14</v>
+        <v>88</v>
       </c>
       <c r="G53" t="s">
         <v>7</v>
       </c>
       <c r="H53" t="s">
-        <v>49</v>
+        <v>31</v>
       </c>
       <c r="I53" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="J53" t="s">
         <v>8</v>
       </c>
       <c r="K53" t="s">
-        <v>35</v>
+        <v>121</v>
       </c>
       <c r="L53" t="s">
         <v>9</v>
       </c>
       <c r="M53" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="N53" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B54" t="s">
         <v>3</v>
@@ -3682,7 +3685,7 @@
         <v>20</v>
       </c>
       <c r="E54">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F54" t="s">
         <v>29</v>
@@ -3691,7 +3694,7 @@
         <v>7</v>
       </c>
       <c r="H54" t="s">
-        <v>55</v>
+        <v>17</v>
       </c>
       <c r="I54" t="s">
         <v>9</v>
@@ -3700,10 +3703,10 @@
         <v>8</v>
       </c>
       <c r="K54" t="s">
-        <v>57</v>
+        <v>123</v>
       </c>
       <c r="L54" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="M54" t="s">
         <v>8</v>
@@ -3712,9 +3715,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B55" t="s">
         <v>3</v>
@@ -3723,10 +3726,10 @@
         <v>4</v>
       </c>
       <c r="D55" t="s">
-        <v>20</v>
+        <v>97</v>
       </c>
       <c r="E55">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F55" t="s">
         <v>88</v>
@@ -3735,7 +3738,7 @@
         <v>7</v>
       </c>
       <c r="H55" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="I55" t="s">
         <v>9</v>
@@ -3744,21 +3747,21 @@
         <v>8</v>
       </c>
       <c r="K55" t="s">
-        <v>123</v>
+        <v>57</v>
       </c>
       <c r="L55" t="s">
         <v>9</v>
       </c>
       <c r="M55" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="N55" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B56" t="s">
         <v>3</v>
@@ -3773,13 +3776,13 @@
         <v>8</v>
       </c>
       <c r="F56" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="G56" t="s">
         <v>7</v>
       </c>
       <c r="H56" t="s">
-        <v>17</v>
+        <v>49</v>
       </c>
       <c r="I56" t="s">
         <v>9</v>
@@ -3788,7 +3791,7 @@
         <v>8</v>
       </c>
       <c r="K56" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="L56" t="s">
         <v>9</v>
@@ -3800,9 +3803,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B57" t="s">
         <v>3</v>
@@ -3814,7 +3817,7 @@
         <v>20</v>
       </c>
       <c r="E57">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F57" t="s">
         <v>14</v>
@@ -3832,7 +3835,7 @@
         <v>27</v>
       </c>
       <c r="K57" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="L57" t="s">
         <v>15</v>
@@ -3844,9 +3847,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B58" t="s">
         <v>3</v>
@@ -3858,16 +3861,16 @@
         <v>5</v>
       </c>
       <c r="E58">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F58" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="G58" t="s">
-        <v>44</v>
+        <v>7</v>
       </c>
       <c r="H58" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="I58" t="s">
         <v>9</v>
@@ -3876,7 +3879,7 @@
         <v>8</v>
       </c>
       <c r="K58" t="s">
-        <v>57</v>
+        <v>129</v>
       </c>
       <c r="L58" t="s">
         <v>9</v>
@@ -3888,9 +3891,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B59" t="s">
         <v>3</v>
@@ -3905,13 +3908,13 @@
         <v>5</v>
       </c>
       <c r="F59" t="s">
-        <v>88</v>
+        <v>14</v>
       </c>
       <c r="G59" t="s">
         <v>7</v>
       </c>
       <c r="H59" t="s">
-        <v>17</v>
+        <v>45</v>
       </c>
       <c r="I59" t="s">
         <v>9</v>
@@ -3920,7 +3923,7 @@
         <v>8</v>
       </c>
       <c r="K59" t="s">
-        <v>57</v>
+        <v>129</v>
       </c>
       <c r="L59" t="s">
         <v>9</v>
@@ -3932,40 +3935,40 @@
         <v>13</v>
       </c>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
+        <v>131</v>
+      </c>
+      <c r="B60" t="s">
+        <v>3</v>
+      </c>
+      <c r="C60" t="s">
+        <v>4</v>
+      </c>
+      <c r="D60" t="s">
+        <v>20</v>
+      </c>
+      <c r="E60">
+        <v>5</v>
+      </c>
+      <c r="F60" t="s">
+        <v>14</v>
+      </c>
+      <c r="G60" t="s">
+        <v>7</v>
+      </c>
+      <c r="H60" t="s">
+        <v>45</v>
+      </c>
+      <c r="I60" t="s">
+        <v>9</v>
+      </c>
+      <c r="J60" t="s">
+        <v>8</v>
+      </c>
+      <c r="K60" t="s">
         <v>129</v>
       </c>
-      <c r="B60" t="s">
-        <v>3</v>
-      </c>
-      <c r="C60" t="s">
-        <v>4</v>
-      </c>
-      <c r="D60" t="s">
-        <v>20</v>
-      </c>
-      <c r="E60">
-        <v>8</v>
-      </c>
-      <c r="F60" t="s">
-        <v>54</v>
-      </c>
-      <c r="G60" t="s">
-        <v>7</v>
-      </c>
-      <c r="H60" t="s">
-        <v>49</v>
-      </c>
-      <c r="I60" t="s">
-        <v>9</v>
-      </c>
-      <c r="J60" t="s">
-        <v>8</v>
-      </c>
-      <c r="K60" t="s">
-        <v>130</v>
-      </c>
       <c r="L60" t="s">
         <v>9</v>
       </c>
@@ -3976,9 +3979,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B61" t="s">
         <v>3</v>
@@ -3999,30 +4002,30 @@
         <v>7</v>
       </c>
       <c r="H61" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="I61" t="s">
         <v>9</v>
       </c>
       <c r="J61" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="K61" t="s">
-        <v>68</v>
+        <v>39</v>
       </c>
       <c r="L61" t="s">
         <v>15</v>
       </c>
       <c r="M61" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="N61" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B62" t="s">
         <v>3</v>
@@ -4031,19 +4034,19 @@
         <v>4</v>
       </c>
       <c r="D62" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="E62">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="F62" t="s">
-        <v>14</v>
+        <v>54</v>
       </c>
       <c r="G62" t="s">
-        <v>7</v>
+        <v>44</v>
       </c>
       <c r="H62" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="I62" t="s">
         <v>9</v>
@@ -4052,10 +4055,10 @@
         <v>8</v>
       </c>
       <c r="K62" t="s">
-        <v>133</v>
+        <v>33</v>
       </c>
       <c r="L62" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="M62" t="s">
         <v>8</v>
@@ -4064,7 +4067,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>134</v>
       </c>
@@ -4096,10 +4099,10 @@
         <v>8</v>
       </c>
       <c r="K63" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="L63" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="M63" t="s">
         <v>8</v>
@@ -4108,7 +4111,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>135</v>
       </c>
@@ -4119,10 +4122,10 @@
         <v>4</v>
       </c>
       <c r="D64" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="E64">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F64" t="s">
         <v>14</v>
@@ -4131,7 +4134,7 @@
         <v>7</v>
       </c>
       <c r="H64" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="I64" t="s">
         <v>9</v>
@@ -4140,7 +4143,7 @@
         <v>8</v>
       </c>
       <c r="K64" t="s">
-        <v>133</v>
+        <v>57</v>
       </c>
       <c r="L64" t="s">
         <v>9</v>
@@ -4152,7 +4155,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>136</v>
       </c>
@@ -4163,10 +4166,10 @@
         <v>4</v>
       </c>
       <c r="D65" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="E65">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="F65" t="s">
         <v>14</v>
@@ -4175,7 +4178,7 @@
         <v>7</v>
       </c>
       <c r="H65" t="s">
-        <v>17</v>
+        <v>45</v>
       </c>
       <c r="I65" t="s">
         <v>9</v>
@@ -4184,19 +4187,19 @@
         <v>8</v>
       </c>
       <c r="K65" t="s">
-        <v>39</v>
+        <v>129</v>
       </c>
       <c r="L65" t="s">
         <v>15</v>
       </c>
       <c r="M65" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="N65" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>137</v>
       </c>
@@ -4207,28 +4210,28 @@
         <v>4</v>
       </c>
       <c r="D66" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="E66">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="F66" t="s">
-        <v>54</v>
+        <v>14</v>
       </c>
       <c r="G66" t="s">
-        <v>44</v>
+        <v>7</v>
       </c>
       <c r="H66" t="s">
-        <v>17</v>
+        <v>45</v>
       </c>
       <c r="I66" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="J66" t="s">
         <v>8</v>
       </c>
       <c r="K66" t="s">
-        <v>33</v>
+        <v>129</v>
       </c>
       <c r="L66" t="s">
         <v>15</v>
@@ -4240,7 +4243,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>138</v>
       </c>
@@ -4266,13 +4269,13 @@
         <v>45</v>
       </c>
       <c r="I67" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="J67" t="s">
         <v>8</v>
       </c>
       <c r="K67" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="L67" t="s">
         <v>15</v>
@@ -4284,7 +4287,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>139</v>
       </c>
@@ -4295,42 +4298,42 @@
         <v>4</v>
       </c>
       <c r="D68" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="E68">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="F68" t="s">
         <v>14</v>
       </c>
       <c r="G68" t="s">
-        <v>7</v>
+        <v>37</v>
       </c>
       <c r="H68" t="s">
-        <v>31</v>
+        <v>140</v>
       </c>
       <c r="I68" t="s">
         <v>9</v>
       </c>
       <c r="J68" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="K68" t="s">
-        <v>57</v>
+        <v>10</v>
       </c>
       <c r="L68" t="s">
         <v>9</v>
       </c>
       <c r="M68" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="N68" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B69" t="s">
         <v>3</v>
@@ -4339,19 +4342,19 @@
         <v>4</v>
       </c>
       <c r="D69" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="E69">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="F69" t="s">
-        <v>14</v>
+        <v>88</v>
       </c>
       <c r="G69" t="s">
         <v>7</v>
       </c>
       <c r="H69" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
       <c r="I69" t="s">
         <v>9</v>
@@ -4360,10 +4363,10 @@
         <v>8</v>
       </c>
       <c r="K69" t="s">
-        <v>133</v>
+        <v>142</v>
       </c>
       <c r="L69" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="M69" t="s">
         <v>8</v>
@@ -4372,9 +4375,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B70" t="s">
         <v>3</v>
@@ -4383,28 +4386,28 @@
         <v>4</v>
       </c>
       <c r="D70" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="E70">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="F70" t="s">
-        <v>14</v>
+        <v>54</v>
       </c>
       <c r="G70" t="s">
-        <v>7</v>
+        <v>44</v>
       </c>
       <c r="H70" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
       <c r="I70" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="J70" t="s">
         <v>8</v>
       </c>
       <c r="K70" t="s">
-        <v>133</v>
+        <v>144</v>
       </c>
       <c r="L70" t="s">
         <v>15</v>
@@ -4416,9 +4419,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="B71" t="s">
         <v>3</v>
@@ -4427,10 +4430,10 @@
         <v>4</v>
       </c>
       <c r="D71" t="s">
-        <v>97</v>
+        <v>20</v>
       </c>
       <c r="E71">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F71" t="s">
         <v>14</v>
@@ -4439,68 +4442,24 @@
         <v>7</v>
       </c>
       <c r="H71" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="I71" t="s">
         <v>15</v>
       </c>
       <c r="J71" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="K71" t="s">
-        <v>133</v>
+        <v>10</v>
       </c>
       <c r="L71" t="s">
         <v>15</v>
       </c>
       <c r="M71" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="N71" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
-        <v>143</v>
-      </c>
-      <c r="B72" t="s">
-        <v>3</v>
-      </c>
-      <c r="C72" t="s">
-        <v>4</v>
-      </c>
-      <c r="D72" t="s">
-        <v>20</v>
-      </c>
-      <c r="E72">
-        <v>8</v>
-      </c>
-      <c r="F72" t="s">
-        <v>14</v>
-      </c>
-      <c r="G72" t="s">
-        <v>37</v>
-      </c>
-      <c r="H72" t="s">
-        <v>144</v>
-      </c>
-      <c r="I72" t="s">
-        <v>9</v>
-      </c>
-      <c r="J72" t="s">
-        <v>27</v>
-      </c>
-      <c r="K72" t="s">
-        <v>10</v>
-      </c>
-      <c r="L72" t="s">
-        <v>9</v>
-      </c>
-      <c r="M72" t="s">
-        <v>27</v>
-      </c>
-      <c r="N72" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Removed set 1 due to multiple beacon devices
</commit_message>
<xml_diff>
--- a/Index.xlsx
+++ b/Index.xlsx
@@ -1,29 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mkrangle\Documents\Projects\PACT\PACT Submissions\Range Angle Structured\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F719CB73-F18D-46D9-AE4D-CE8FDC86A705}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B906AB1-B44B-4189-B1E4-E2AB45EEFC23}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2130" yWindow="2505" windowWidth="27285" windowHeight="14010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="12615" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index_structured" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">index_structured!$A$1:$P$30</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">index_structured!$A$1:$P$29</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="924" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="911" uniqueCount="145">
   <si>
     <t>environment_1</t>
   </si>
@@ -95,9 +95,6 @@
   </si>
   <si>
     <t xml:space="preserve"> iPhone XR</t>
-  </si>
-  <si>
-    <t>set_1</t>
   </si>
   <si>
     <t>shirt pocket</t>
@@ -1318,74 +1315,74 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N71"/>
+  <dimension ref="A1:N70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="A72" sqref="A72:XFD72"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.453125" customWidth="1"/>
-    <col min="3" max="3" width="13.453125" customWidth="1"/>
-    <col min="4" max="4" width="28.54296875" customWidth="1"/>
-    <col min="6" max="6" width="15.453125" customWidth="1"/>
-    <col min="7" max="7" width="20.54296875" customWidth="1"/>
-    <col min="8" max="9" width="15.453125" customWidth="1"/>
-    <col min="10" max="10" width="20.54296875" customWidth="1"/>
-    <col min="11" max="11" width="19.1796875" customWidth="1"/>
-    <col min="12" max="12" width="15.453125" customWidth="1"/>
-    <col min="13" max="13" width="20.54296875" customWidth="1"/>
-    <col min="14" max="14" width="15.453125" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" customWidth="1"/>
+    <col min="4" max="4" width="28.5703125" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" customWidth="1"/>
+    <col min="7" max="7" width="20.5703125" customWidth="1"/>
+    <col min="8" max="9" width="15.42578125" customWidth="1"/>
+    <col min="10" max="10" width="20.5703125" customWidth="1"/>
+    <col min="11" max="11" width="19.140625" customWidth="1"/>
+    <col min="12" max="12" width="15.42578125" customWidth="1"/>
+    <col min="13" max="13" width="20.5703125" customWidth="1"/>
+    <col min="14" max="14" width="15.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:14" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>77</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>78</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="H1" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="M1" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="I1" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="L1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="M1" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>68</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
@@ -1400,13 +1397,13 @@
         <v>8</v>
       </c>
       <c r="F2" t="s">
-        <v>14</v>
+        <v>53</v>
       </c>
       <c r="G2" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="H2" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="I2" t="s">
         <v>9</v>
@@ -1415,7 +1412,7 @@
         <v>8</v>
       </c>
       <c r="K2" t="s">
-        <v>22</v>
+        <v>67</v>
       </c>
       <c r="L2" t="s">
         <v>15</v>
@@ -1427,9 +1424,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>69</v>
+        <v>47</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
@@ -1444,13 +1441,13 @@
         <v>8</v>
       </c>
       <c r="F3" t="s">
-        <v>54</v>
+        <v>14</v>
       </c>
       <c r="G3" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="H3" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="I3" t="s">
         <v>9</v>
@@ -1459,21 +1456,21 @@
         <v>8</v>
       </c>
       <c r="K3" t="s">
-        <v>68</v>
+        <v>25</v>
       </c>
       <c r="L3" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="M3" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="N3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>48</v>
+        <v>66</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
@@ -1488,36 +1485,36 @@
         <v>8</v>
       </c>
       <c r="F4" t="s">
-        <v>14</v>
+        <v>53</v>
       </c>
       <c r="G4" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="H4" t="s">
         <v>23</v>
       </c>
       <c r="I4" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="J4" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="K4" t="s">
+        <v>56</v>
+      </c>
+      <c r="L4" t="s">
+        <v>9</v>
+      </c>
+      <c r="M4" t="s">
         <v>26</v>
       </c>
-      <c r="L4" t="s">
-        <v>9</v>
-      </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>27</v>
-      </c>
-      <c r="N4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>67</v>
       </c>
       <c r="B5" t="s">
         <v>3</v>
@@ -1532,7 +1529,7 @@
         <v>8</v>
       </c>
       <c r="F5" t="s">
-        <v>54</v>
+        <v>14</v>
       </c>
       <c r="G5" t="s">
         <v>7</v>
@@ -1541,27 +1538,27 @@
         <v>23</v>
       </c>
       <c r="I5" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="J5" t="s">
+        <v>24</v>
+      </c>
+      <c r="K5" t="s">
         <v>25</v>
       </c>
-      <c r="K5" t="s">
-        <v>57</v>
-      </c>
       <c r="L5" t="s">
         <v>9</v>
       </c>
       <c r="M5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B6" t="s">
         <v>3</v>
@@ -1576,80 +1573,80 @@
         <v>8</v>
       </c>
       <c r="F6" t="s">
+        <v>28</v>
+      </c>
+      <c r="G6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H6" t="s">
+        <v>30</v>
+      </c>
+      <c r="I6" t="s">
+        <v>9</v>
+      </c>
+      <c r="J6" t="s">
+        <v>26</v>
+      </c>
+      <c r="K6" t="s">
+        <v>29</v>
+      </c>
+      <c r="L6" t="s">
+        <v>9</v>
+      </c>
+      <c r="M6" t="s">
+        <v>26</v>
+      </c>
+      <c r="N6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7">
+        <v>7</v>
+      </c>
+      <c r="F7" t="s">
         <v>14</v>
       </c>
-      <c r="G6" t="s">
-        <v>7</v>
-      </c>
-      <c r="H6" t="s">
-        <v>23</v>
-      </c>
-      <c r="I6" t="s">
-        <v>9</v>
-      </c>
-      <c r="J6" t="s">
-        <v>25</v>
-      </c>
-      <c r="K6" t="s">
+      <c r="G7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I7" t="s">
+        <v>9</v>
+      </c>
+      <c r="J7" t="s">
         <v>26</v>
       </c>
-      <c r="L6" t="s">
-        <v>9</v>
-      </c>
-      <c r="M6" t="s">
-        <v>27</v>
-      </c>
-      <c r="N6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>32</v>
-      </c>
-      <c r="B7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" t="s">
-        <v>20</v>
-      </c>
-      <c r="E7">
-        <v>8</v>
-      </c>
-      <c r="F7" t="s">
-        <v>29</v>
-      </c>
-      <c r="G7" t="s">
-        <v>7</v>
-      </c>
-      <c r="H7" t="s">
-        <v>31</v>
-      </c>
-      <c r="I7" t="s">
-        <v>9</v>
-      </c>
-      <c r="J7" t="s">
-        <v>27</v>
-      </c>
       <c r="K7" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="L7" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="M7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B8" t="s">
         <v>3</v>
@@ -1658,107 +1655,107 @@
         <v>4</v>
       </c>
       <c r="D8" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="E8">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="F8" t="s">
         <v>14</v>
       </c>
       <c r="G8" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="H8" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="I8" t="s">
         <v>9</v>
       </c>
       <c r="J8" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="K8" t="s">
-        <v>39</v>
+        <v>56</v>
       </c>
       <c r="L8" t="s">
+        <v>9</v>
+      </c>
+      <c r="M8" t="s">
+        <v>8</v>
+      </c>
+      <c r="N8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>49</v>
+      </c>
+      <c r="B9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9">
+        <v>8</v>
+      </c>
+      <c r="F9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G9" t="s">
+        <v>7</v>
+      </c>
+      <c r="H9" t="s">
+        <v>48</v>
+      </c>
+      <c r="I9" t="s">
+        <v>9</v>
+      </c>
+      <c r="J9" t="s">
+        <v>8</v>
+      </c>
+      <c r="K9" t="s">
+        <v>10</v>
+      </c>
+      <c r="L9" t="s">
         <v>15</v>
       </c>
-      <c r="M8" t="s">
-        <v>27</v>
-      </c>
-      <c r="N8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>64</v>
-      </c>
-      <c r="B9" t="s">
-        <v>3</v>
-      </c>
-      <c r="C9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D9" t="s">
-        <v>5</v>
-      </c>
-      <c r="E9">
-        <v>2</v>
-      </c>
-      <c r="F9" t="s">
+      <c r="M9" t="s">
+        <v>8</v>
+      </c>
+      <c r="N9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>61</v>
+      </c>
+      <c r="B10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10">
+        <v>8</v>
+      </c>
+      <c r="F10" t="s">
         <v>14</v>
       </c>
-      <c r="G9" t="s">
-        <v>44</v>
-      </c>
-      <c r="H9" t="s">
-        <v>23</v>
-      </c>
-      <c r="I9" t="s">
-        <v>9</v>
-      </c>
-      <c r="J9" t="s">
-        <v>8</v>
-      </c>
-      <c r="K9" t="s">
-        <v>57</v>
-      </c>
-      <c r="L9" t="s">
-        <v>9</v>
-      </c>
-      <c r="M9" t="s">
-        <v>8</v>
-      </c>
-      <c r="N9" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>50</v>
-      </c>
-      <c r="B10" t="s">
-        <v>3</v>
-      </c>
-      <c r="C10" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" t="s">
-        <v>20</v>
-      </c>
-      <c r="E10">
-        <v>8</v>
-      </c>
-      <c r="F10" t="s">
-        <v>29</v>
-      </c>
       <c r="G10" t="s">
         <v>7</v>
       </c>
       <c r="H10" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="I10" t="s">
         <v>9</v>
@@ -1767,7 +1764,7 @@
         <v>8</v>
       </c>
       <c r="K10" t="s">
-        <v>10</v>
+        <v>56</v>
       </c>
       <c r="L10" t="s">
         <v>15</v>
@@ -1779,9 +1776,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>62</v>
+        <v>72</v>
       </c>
       <c r="B11" t="s">
         <v>3</v>
@@ -1802,7 +1799,7 @@
         <v>7</v>
       </c>
       <c r="H11" t="s">
-        <v>61</v>
+        <v>11</v>
       </c>
       <c r="I11" t="s">
         <v>9</v>
@@ -1811,10 +1808,10 @@
         <v>8</v>
       </c>
       <c r="K11" t="s">
-        <v>57</v>
+        <v>25</v>
       </c>
       <c r="L11" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="M11" t="s">
         <v>8</v>
@@ -1823,9 +1820,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>73</v>
+        <v>35</v>
       </c>
       <c r="B12" t="s">
         <v>3</v>
@@ -1843,121 +1840,121 @@
         <v>14</v>
       </c>
       <c r="G12" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="H12" t="s">
+        <v>23</v>
+      </c>
+      <c r="I12" t="s">
+        <v>9</v>
+      </c>
+      <c r="J12" t="s">
+        <v>8</v>
+      </c>
+      <c r="K12" t="s">
+        <v>34</v>
+      </c>
+      <c r="L12" t="s">
+        <v>9</v>
+      </c>
+      <c r="M12" t="s">
+        <v>8</v>
+      </c>
+      <c r="N12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>51</v>
+      </c>
+      <c r="B13" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" t="s">
+        <v>20</v>
+      </c>
+      <c r="E13">
+        <v>8</v>
+      </c>
+      <c r="F13" t="s">
+        <v>28</v>
+      </c>
+      <c r="G13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H13" t="s">
+        <v>50</v>
+      </c>
+      <c r="I13" t="s">
+        <v>9</v>
+      </c>
+      <c r="J13" t="s">
+        <v>8</v>
+      </c>
+      <c r="K13" t="s">
+        <v>25</v>
+      </c>
+      <c r="L13" t="s">
+        <v>9</v>
+      </c>
+      <c r="M13" t="s">
+        <v>8</v>
+      </c>
+      <c r="N13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" t="s">
+        <v>20</v>
+      </c>
+      <c r="E14">
+        <v>8</v>
+      </c>
+      <c r="F14" t="s">
+        <v>14</v>
+      </c>
+      <c r="G14" t="s">
+        <v>36</v>
+      </c>
+      <c r="H14" t="s">
         <v>11</v>
       </c>
-      <c r="I12" t="s">
-        <v>9</v>
-      </c>
-      <c r="J12" t="s">
-        <v>8</v>
-      </c>
-      <c r="K12" t="s">
+      <c r="I14" t="s">
+        <v>9</v>
+      </c>
+      <c r="J14" t="s">
+        <v>37</v>
+      </c>
+      <c r="K14" t="s">
+        <v>38</v>
+      </c>
+      <c r="L14" t="s">
+        <v>9</v>
+      </c>
+      <c r="M14" t="s">
         <v>26</v>
       </c>
-      <c r="L12" t="s">
-        <v>9</v>
-      </c>
-      <c r="M12" t="s">
-        <v>8</v>
-      </c>
-      <c r="N12" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>36</v>
-      </c>
-      <c r="B13" t="s">
-        <v>3</v>
-      </c>
-      <c r="C13" t="s">
-        <v>4</v>
-      </c>
-      <c r="D13" t="s">
-        <v>20</v>
-      </c>
-      <c r="E13">
-        <v>8</v>
-      </c>
-      <c r="F13" t="s">
-        <v>14</v>
-      </c>
-      <c r="G13" t="s">
-        <v>21</v>
-      </c>
-      <c r="H13" t="s">
-        <v>23</v>
-      </c>
-      <c r="I13" t="s">
-        <v>9</v>
-      </c>
-      <c r="J13" t="s">
-        <v>8</v>
-      </c>
-      <c r="K13" t="s">
-        <v>35</v>
-      </c>
-      <c r="L13" t="s">
-        <v>9</v>
-      </c>
-      <c r="M13" t="s">
-        <v>8</v>
-      </c>
-      <c r="N13" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>52</v>
-      </c>
-      <c r="B14" t="s">
-        <v>3</v>
-      </c>
-      <c r="C14" t="s">
-        <v>4</v>
-      </c>
-      <c r="D14" t="s">
-        <v>20</v>
-      </c>
-      <c r="E14">
-        <v>8</v>
-      </c>
-      <c r="F14" t="s">
-        <v>29</v>
-      </c>
-      <c r="G14" t="s">
-        <v>7</v>
-      </c>
-      <c r="H14" t="s">
-        <v>51</v>
-      </c>
-      <c r="I14" t="s">
-        <v>9</v>
-      </c>
-      <c r="J14" t="s">
-        <v>8</v>
-      </c>
-      <c r="K14" t="s">
-        <v>26</v>
-      </c>
-      <c r="L14" t="s">
-        <v>9</v>
-      </c>
-      <c r="M14" t="s">
-        <v>8</v>
-      </c>
       <c r="N14" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>40</v>
+        <v>18</v>
       </c>
       <c r="B15" t="s">
         <v>3</v>
@@ -1966,120 +1963,120 @@
         <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="E15">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="F15" t="s">
         <v>14</v>
       </c>
       <c r="G15" t="s">
-        <v>37</v>
+        <v>7</v>
       </c>
       <c r="H15" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="I15" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="J15" t="s">
+        <v>8</v>
+      </c>
+      <c r="K15" t="s">
+        <v>16</v>
+      </c>
+      <c r="L15" t="s">
+        <v>15</v>
+      </c>
+      <c r="M15" t="s">
+        <v>8</v>
+      </c>
+      <c r="N15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16" t="s">
+        <v>20</v>
+      </c>
+      <c r="E16">
+        <v>8</v>
+      </c>
+      <c r="F16" t="s">
+        <v>6</v>
+      </c>
+      <c r="G16" t="s">
+        <v>21</v>
+      </c>
+      <c r="H16" t="s">
+        <v>30</v>
+      </c>
+      <c r="I16" t="s">
+        <v>9</v>
+      </c>
+      <c r="J16" t="s">
+        <v>8</v>
+      </c>
+      <c r="K16" t="s">
+        <v>32</v>
+      </c>
+      <c r="L16" t="s">
+        <v>9</v>
+      </c>
+      <c r="M16" t="s">
+        <v>8</v>
+      </c>
+      <c r="N16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>46</v>
+      </c>
+      <c r="B17" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17" t="s">
+        <v>20</v>
+      </c>
+      <c r="E17">
+        <v>8</v>
+      </c>
+      <c r="F17" t="s">
+        <v>14</v>
+      </c>
+      <c r="G17" t="s">
+        <v>43</v>
+      </c>
+      <c r="H17" t="s">
+        <v>23</v>
+      </c>
+      <c r="I17" t="s">
+        <v>9</v>
+      </c>
+      <c r="J17" t="s">
+        <v>8</v>
+      </c>
+      <c r="K17" t="s">
         <v>38</v>
       </c>
-      <c r="K15" t="s">
-        <v>39</v>
-      </c>
-      <c r="L15" t="s">
-        <v>9</v>
-      </c>
-      <c r="M15" t="s">
-        <v>27</v>
-      </c>
-      <c r="N15" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>18</v>
-      </c>
-      <c r="B16" t="s">
-        <v>3</v>
-      </c>
-      <c r="C16" t="s">
-        <v>4</v>
-      </c>
-      <c r="D16" t="s">
-        <v>5</v>
-      </c>
-      <c r="E16">
-        <v>2</v>
-      </c>
-      <c r="F16" t="s">
-        <v>14</v>
-      </c>
-      <c r="G16" t="s">
-        <v>7</v>
-      </c>
-      <c r="H16" t="s">
-        <v>17</v>
-      </c>
-      <c r="I16" t="s">
+      <c r="L17" t="s">
         <v>15</v>
       </c>
-      <c r="J16" t="s">
-        <v>8</v>
-      </c>
-      <c r="K16" t="s">
-        <v>16</v>
-      </c>
-      <c r="L16" t="s">
-        <v>15</v>
-      </c>
-      <c r="M16" t="s">
-        <v>8</v>
-      </c>
-      <c r="N16" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>34</v>
-      </c>
-      <c r="B17" t="s">
-        <v>3</v>
-      </c>
-      <c r="C17" t="s">
-        <v>4</v>
-      </c>
-      <c r="D17" t="s">
-        <v>20</v>
-      </c>
-      <c r="E17">
-        <v>8</v>
-      </c>
-      <c r="F17" t="s">
-        <v>6</v>
-      </c>
-      <c r="G17" t="s">
-        <v>21</v>
-      </c>
-      <c r="H17" t="s">
-        <v>31</v>
-      </c>
-      <c r="I17" t="s">
-        <v>9</v>
-      </c>
-      <c r="J17" t="s">
-        <v>8</v>
-      </c>
-      <c r="K17" t="s">
-        <v>33</v>
-      </c>
-      <c r="L17" t="s">
-        <v>9</v>
-      </c>
       <c r="M17" t="s">
         <v>8</v>
       </c>
@@ -2087,9 +2084,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>47</v>
+        <v>70</v>
       </c>
       <c r="B18" t="s">
         <v>3</v>
@@ -2107,10 +2104,10 @@
         <v>14</v>
       </c>
       <c r="G18" t="s">
-        <v>44</v>
+        <v>7</v>
       </c>
       <c r="H18" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="I18" t="s">
         <v>9</v>
@@ -2119,10 +2116,10 @@
         <v>8</v>
       </c>
       <c r="K18" t="s">
-        <v>39</v>
+        <v>69</v>
       </c>
       <c r="L18" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="M18" t="s">
         <v>8</v>
@@ -2131,9 +2128,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="B19" t="s">
         <v>3</v>
@@ -2154,7 +2151,7 @@
         <v>7</v>
       </c>
       <c r="H19" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="I19" t="s">
         <v>9</v>
@@ -2163,21 +2160,21 @@
         <v>8</v>
       </c>
       <c r="K19" t="s">
-        <v>70</v>
+        <v>38</v>
       </c>
       <c r="L19" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="M19" t="s">
-        <v>8</v>
+        <v>37</v>
       </c>
       <c r="N19" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B20" t="s">
         <v>3</v>
@@ -2192,13 +2189,13 @@
         <v>8</v>
       </c>
       <c r="F20" t="s">
-        <v>14</v>
+        <v>53</v>
       </c>
       <c r="G20" t="s">
         <v>7</v>
       </c>
       <c r="H20" t="s">
-        <v>23</v>
+        <v>54</v>
       </c>
       <c r="I20" t="s">
         <v>9</v>
@@ -2207,65 +2204,65 @@
         <v>8</v>
       </c>
       <c r="K20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L20" t="s">
         <v>15</v>
       </c>
       <c r="M20" t="s">
+        <v>8</v>
+      </c>
+      <c r="N20" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>74</v>
+      </c>
+      <c r="B21" t="s">
+        <v>3</v>
+      </c>
+      <c r="C21" t="s">
+        <v>4</v>
+      </c>
+      <c r="D21" t="s">
+        <v>20</v>
+      </c>
+      <c r="E21">
+        <v>8</v>
+      </c>
+      <c r="F21" t="s">
+        <v>14</v>
+      </c>
+      <c r="G21" t="s">
+        <v>7</v>
+      </c>
+      <c r="H21" t="s">
+        <v>23</v>
+      </c>
+      <c r="I21" t="s">
+        <v>9</v>
+      </c>
+      <c r="J21" t="s">
+        <v>8</v>
+      </c>
+      <c r="K21" t="s">
         <v>38</v>
-      </c>
-      <c r="N20" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
-        <v>56</v>
-      </c>
-      <c r="B21" t="s">
-        <v>3</v>
-      </c>
-      <c r="C21" t="s">
-        <v>4</v>
-      </c>
-      <c r="D21" t="s">
-        <v>20</v>
-      </c>
-      <c r="E21">
-        <v>8</v>
-      </c>
-      <c r="F21" t="s">
-        <v>54</v>
-      </c>
-      <c r="G21" t="s">
-        <v>7</v>
-      </c>
-      <c r="H21" t="s">
-        <v>55</v>
-      </c>
-      <c r="I21" t="s">
-        <v>9</v>
-      </c>
-      <c r="J21" t="s">
-        <v>8</v>
-      </c>
-      <c r="K21" t="s">
-        <v>39</v>
       </c>
       <c r="L21" t="s">
         <v>15</v>
       </c>
       <c r="M21" t="s">
-        <v>8</v>
+        <v>73</v>
       </c>
       <c r="N21" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B22" t="s">
         <v>3</v>
@@ -2292,24 +2289,24 @@
         <v>9</v>
       </c>
       <c r="J22" t="s">
-        <v>8</v>
+        <v>37</v>
       </c>
       <c r="K22" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L22" t="s">
         <v>15</v>
       </c>
       <c r="M22" t="s">
-        <v>74</v>
+        <v>26</v>
       </c>
       <c r="N22" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="B23" t="s">
         <v>3</v>
@@ -2324,36 +2321,36 @@
         <v>8</v>
       </c>
       <c r="F23" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="G23" t="s">
         <v>7</v>
       </c>
       <c r="H23" t="s">
-        <v>23</v>
+        <v>48</v>
       </c>
       <c r="I23" t="s">
         <v>9</v>
       </c>
       <c r="J23" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="K23" t="s">
-        <v>39</v>
+        <v>10</v>
       </c>
       <c r="L23" t="s">
         <v>15</v>
       </c>
       <c r="M23" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="N23" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="B24" t="s">
         <v>3</v>
@@ -2362,31 +2359,31 @@
         <v>4</v>
       </c>
       <c r="D24" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="E24">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="F24" t="s">
-        <v>29</v>
+        <v>53</v>
       </c>
       <c r="G24" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="H24" t="s">
-        <v>49</v>
+        <v>23</v>
       </c>
       <c r="I24" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="J24" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K24" t="s">
-        <v>10</v>
+        <v>56</v>
       </c>
       <c r="L24" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="M24" t="s">
         <v>8</v>
@@ -2395,9 +2392,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>58</v>
+        <v>12</v>
       </c>
       <c r="B25" t="s">
         <v>3</v>
@@ -2412,22 +2409,22 @@
         <v>2</v>
       </c>
       <c r="F25" t="s">
-        <v>54</v>
+        <v>6</v>
       </c>
       <c r="G25" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="H25" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="I25" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="J25" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="K25" t="s">
-        <v>57</v>
+        <v>10</v>
       </c>
       <c r="L25" t="s">
         <v>9</v>
@@ -2439,9 +2436,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>12</v>
+        <v>65</v>
       </c>
       <c r="B26" t="s">
         <v>3</v>
@@ -2450,19 +2447,19 @@
         <v>4</v>
       </c>
       <c r="D26" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="E26">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="F26" t="s">
         <v>6</v>
       </c>
       <c r="G26" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="H26" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="I26" t="s">
         <v>9</v>
@@ -2471,21 +2468,21 @@
         <v>8</v>
       </c>
       <c r="K26" t="s">
-        <v>10</v>
+        <v>64</v>
       </c>
       <c r="L26" t="s">
         <v>9</v>
       </c>
       <c r="M26" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="N26" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="B27" t="s">
         <v>3</v>
@@ -2500,13 +2497,13 @@
         <v>8</v>
       </c>
       <c r="F27" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="G27" t="s">
-        <v>44</v>
+        <v>7</v>
       </c>
       <c r="H27" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="I27" t="s">
         <v>9</v>
@@ -2515,21 +2512,21 @@
         <v>8</v>
       </c>
       <c r="K27" t="s">
-        <v>65</v>
+        <v>38</v>
       </c>
       <c r="L27" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="M27" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N27" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="B28" t="s">
         <v>3</v>
@@ -2550,74 +2547,74 @@
         <v>7</v>
       </c>
       <c r="H28" t="s">
-        <v>23</v>
+        <v>41</v>
       </c>
       <c r="I28" t="s">
         <v>9</v>
       </c>
       <c r="J28" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="K28" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="L28" t="s">
         <v>15</v>
       </c>
       <c r="M28" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N28" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>45</v>
+      </c>
+      <c r="B29" t="s">
+        <v>3</v>
+      </c>
+      <c r="C29" t="s">
+        <v>4</v>
+      </c>
+      <c r="D29" t="s">
+        <v>5</v>
+      </c>
+      <c r="E29">
+        <v>2</v>
+      </c>
+      <c r="F29" t="s">
+        <v>6</v>
+      </c>
+      <c r="G29" t="s">
         <v>43</v>
       </c>
-      <c r="B29" t="s">
-        <v>3</v>
-      </c>
-      <c r="C29" t="s">
-        <v>4</v>
-      </c>
-      <c r="D29" t="s">
-        <v>20</v>
-      </c>
-      <c r="E29">
-        <v>8</v>
-      </c>
-      <c r="F29" t="s">
-        <v>14</v>
-      </c>
-      <c r="G29" t="s">
-        <v>7</v>
-      </c>
       <c r="H29" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="I29" t="s">
         <v>9</v>
       </c>
       <c r="J29" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="K29" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="L29" t="s">
         <v>15</v>
       </c>
       <c r="M29" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="N29" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>46</v>
+        <v>86</v>
       </c>
       <c r="B30" t="s">
         <v>3</v>
@@ -2626,19 +2623,19 @@
         <v>4</v>
       </c>
       <c r="D30" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="E30">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="F30" t="s">
-        <v>6</v>
+        <v>87</v>
       </c>
       <c r="G30" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H30" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
       <c r="I30" t="s">
         <v>9</v>
@@ -2647,10 +2644,10 @@
         <v>8</v>
       </c>
       <c r="K30" t="s">
-        <v>26</v>
+        <v>88</v>
       </c>
       <c r="L30" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="M30" t="s">
         <v>8</v>
@@ -2659,9 +2656,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B31" t="s">
         <v>3</v>
@@ -2676,13 +2673,13 @@
         <v>8</v>
       </c>
       <c r="F31" t="s">
-        <v>88</v>
+        <v>14</v>
       </c>
       <c r="G31" t="s">
-        <v>44</v>
+        <v>21</v>
       </c>
       <c r="H31" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="I31" t="s">
         <v>9</v>
@@ -2691,7 +2688,7 @@
         <v>8</v>
       </c>
       <c r="K31" t="s">
-        <v>89</v>
+        <v>16</v>
       </c>
       <c r="L31" t="s">
         <v>9</v>
@@ -2703,7 +2700,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>90</v>
       </c>
@@ -2720,102 +2717,102 @@
         <v>8</v>
       </c>
       <c r="F32" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="G32" t="s">
+        <v>43</v>
+      </c>
+      <c r="H32" t="s">
+        <v>23</v>
+      </c>
+      <c r="I32" t="s">
+        <v>15</v>
+      </c>
+      <c r="J32" t="s">
+        <v>26</v>
+      </c>
+      <c r="K32" t="s">
+        <v>91</v>
+      </c>
+      <c r="L32" t="s">
+        <v>9</v>
+      </c>
+      <c r="M32" t="s">
+        <v>8</v>
+      </c>
+      <c r="N32" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>92</v>
+      </c>
+      <c r="B33" t="s">
+        <v>3</v>
+      </c>
+      <c r="C33" t="s">
+        <v>4</v>
+      </c>
+      <c r="D33" t="s">
+        <v>20</v>
+      </c>
+      <c r="E33">
+        <v>8</v>
+      </c>
+      <c r="F33" t="s">
+        <v>87</v>
+      </c>
+      <c r="G33" t="s">
+        <v>7</v>
+      </c>
+      <c r="H33" t="s">
+        <v>17</v>
+      </c>
+      <c r="I33" t="s">
+        <v>9</v>
+      </c>
+      <c r="J33" t="s">
+        <v>8</v>
+      </c>
+      <c r="K33" t="s">
+        <v>93</v>
+      </c>
+      <c r="L33" t="s">
+        <v>15</v>
+      </c>
+      <c r="M33" t="s">
+        <v>8</v>
+      </c>
+      <c r="N33" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>94</v>
+      </c>
+      <c r="B34" t="s">
+        <v>3</v>
+      </c>
+      <c r="C34" t="s">
+        <v>4</v>
+      </c>
+      <c r="D34" t="s">
+        <v>20</v>
+      </c>
+      <c r="E34">
+        <v>8</v>
+      </c>
+      <c r="F34" t="s">
+        <v>53</v>
+      </c>
+      <c r="G34" t="s">
         <v>21</v>
       </c>
-      <c r="H32" t="s">
-        <v>17</v>
-      </c>
-      <c r="I32" t="s">
-        <v>9</v>
-      </c>
-      <c r="J32" t="s">
-        <v>8</v>
-      </c>
-      <c r="K32" t="s">
-        <v>16</v>
-      </c>
-      <c r="L32" t="s">
-        <v>9</v>
-      </c>
-      <c r="M32" t="s">
-        <v>8</v>
-      </c>
-      <c r="N32" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A33" t="s">
-        <v>91</v>
-      </c>
-      <c r="B33" t="s">
-        <v>3</v>
-      </c>
-      <c r="C33" t="s">
-        <v>4</v>
-      </c>
-      <c r="D33" t="s">
-        <v>20</v>
-      </c>
-      <c r="E33">
-        <v>8</v>
-      </c>
-      <c r="F33" t="s">
-        <v>6</v>
-      </c>
-      <c r="G33" t="s">
-        <v>44</v>
-      </c>
-      <c r="H33" t="s">
+      <c r="H34" t="s">
         <v>23</v>
       </c>
-      <c r="I33" t="s">
-        <v>15</v>
-      </c>
-      <c r="J33" t="s">
-        <v>27</v>
-      </c>
-      <c r="K33" t="s">
-        <v>92</v>
-      </c>
-      <c r="L33" t="s">
-        <v>9</v>
-      </c>
-      <c r="M33" t="s">
-        <v>8</v>
-      </c>
-      <c r="N33" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A34" t="s">
-        <v>93</v>
-      </c>
-      <c r="B34" t="s">
-        <v>3</v>
-      </c>
-      <c r="C34" t="s">
-        <v>4</v>
-      </c>
-      <c r="D34" t="s">
-        <v>20</v>
-      </c>
-      <c r="E34">
-        <v>8</v>
-      </c>
-      <c r="F34" t="s">
-        <v>88</v>
-      </c>
-      <c r="G34" t="s">
-        <v>7</v>
-      </c>
-      <c r="H34" t="s">
-        <v>17</v>
-      </c>
       <c r="I34" t="s">
         <v>9</v>
       </c>
@@ -2823,7 +2820,7 @@
         <v>8</v>
       </c>
       <c r="K34" t="s">
-        <v>94</v>
+        <v>22</v>
       </c>
       <c r="L34" t="s">
         <v>15</v>
@@ -2835,7 +2832,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>95</v>
       </c>
@@ -2846,28 +2843,28 @@
         <v>4</v>
       </c>
       <c r="D35" t="s">
-        <v>20</v>
+        <v>96</v>
       </c>
       <c r="E35">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F35" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G35" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="H35" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="I35" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="J35" t="s">
         <v>8</v>
       </c>
       <c r="K35" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="L35" t="s">
         <v>15</v>
@@ -2879,9 +2876,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B36" t="s">
         <v>3</v>
@@ -2890,84 +2887,84 @@
         <v>4</v>
       </c>
       <c r="D36" t="s">
-        <v>97</v>
+        <v>20</v>
       </c>
       <c r="E36">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F36" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G36" t="s">
         <v>7</v>
       </c>
       <c r="H36" t="s">
+        <v>11</v>
+      </c>
+      <c r="I36" t="s">
+        <v>9</v>
+      </c>
+      <c r="J36" t="s">
+        <v>26</v>
+      </c>
+      <c r="K36" t="s">
+        <v>98</v>
+      </c>
+      <c r="L36" t="s">
+        <v>9</v>
+      </c>
+      <c r="M36" t="s">
+        <v>26</v>
+      </c>
+      <c r="N36" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>99</v>
+      </c>
+      <c r="B37" t="s">
+        <v>3</v>
+      </c>
+      <c r="C37" t="s">
+        <v>4</v>
+      </c>
+      <c r="D37" t="s">
+        <v>20</v>
+      </c>
+      <c r="E37">
+        <v>8</v>
+      </c>
+      <c r="F37" t="s">
+        <v>53</v>
+      </c>
+      <c r="G37" t="s">
+        <v>43</v>
+      </c>
+      <c r="H37" t="s">
         <v>17</v>
       </c>
-      <c r="I36" t="s">
+      <c r="I37" t="s">
+        <v>9</v>
+      </c>
+      <c r="J37" t="s">
+        <v>8</v>
+      </c>
+      <c r="K37" t="s">
+        <v>25</v>
+      </c>
+      <c r="L37" t="s">
         <v>15</v>
       </c>
-      <c r="J36" t="s">
-        <v>8</v>
-      </c>
-      <c r="K36" t="s">
-        <v>39</v>
-      </c>
-      <c r="L36" t="s">
-        <v>15</v>
-      </c>
-      <c r="M36" t="s">
-        <v>8</v>
-      </c>
-      <c r="N36" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A37" t="s">
-        <v>98</v>
-      </c>
-      <c r="B37" t="s">
-        <v>3</v>
-      </c>
-      <c r="C37" t="s">
-        <v>4</v>
-      </c>
-      <c r="D37" t="s">
-        <v>20</v>
-      </c>
-      <c r="E37">
-        <v>8</v>
-      </c>
-      <c r="F37" t="s">
-        <v>54</v>
-      </c>
-      <c r="G37" t="s">
-        <v>7</v>
-      </c>
-      <c r="H37" t="s">
-        <v>11</v>
-      </c>
-      <c r="I37" t="s">
-        <v>9</v>
-      </c>
-      <c r="J37" t="s">
-        <v>27</v>
-      </c>
-      <c r="K37" t="s">
-        <v>99</v>
-      </c>
-      <c r="L37" t="s">
-        <v>9</v>
-      </c>
       <c r="M37" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N37" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>100</v>
       </c>
@@ -2981,37 +2978,37 @@
         <v>20</v>
       </c>
       <c r="E38">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F38" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G38" t="s">
-        <v>44</v>
+        <v>7</v>
       </c>
       <c r="H38" t="s">
-        <v>17</v>
+        <v>60</v>
       </c>
       <c r="I38" t="s">
         <v>9</v>
       </c>
       <c r="J38" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="K38" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="L38" t="s">
         <v>15</v>
       </c>
       <c r="M38" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="N38" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>101</v>
       </c>
@@ -3025,37 +3022,37 @@
         <v>20</v>
       </c>
       <c r="E39">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F39" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G39" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="H39" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="I39" t="s">
         <v>9</v>
       </c>
       <c r="J39" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="K39" t="s">
-        <v>35</v>
+        <v>10</v>
       </c>
       <c r="L39" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="M39" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="N39" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>102</v>
       </c>
@@ -3072,34 +3069,34 @@
         <v>8</v>
       </c>
       <c r="F40" t="s">
-        <v>54</v>
+        <v>14</v>
       </c>
       <c r="G40" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H40" t="s">
-        <v>49</v>
+        <v>17</v>
       </c>
       <c r="I40" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="J40" t="s">
         <v>8</v>
       </c>
       <c r="K40" t="s">
-        <v>10</v>
+        <v>38</v>
       </c>
       <c r="L40" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="M40" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="N40" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>103</v>
       </c>
@@ -3116,25 +3113,25 @@
         <v>8</v>
       </c>
       <c r="F41" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="G41" t="s">
-        <v>44</v>
+        <v>21</v>
       </c>
       <c r="H41" t="s">
         <v>17</v>
       </c>
       <c r="I41" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="J41" t="s">
         <v>8</v>
       </c>
       <c r="K41" t="s">
-        <v>39</v>
+        <v>104</v>
       </c>
       <c r="L41" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="M41" t="s">
         <v>8</v>
@@ -3143,9 +3140,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B42" t="s">
         <v>3</v>
@@ -3160,22 +3157,22 @@
         <v>8</v>
       </c>
       <c r="F42" t="s">
-        <v>6</v>
+        <v>87</v>
       </c>
       <c r="G42" t="s">
-        <v>21</v>
+        <v>43</v>
       </c>
       <c r="H42" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="I42" t="s">
         <v>9</v>
       </c>
       <c r="J42" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="K42" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="L42" t="s">
         <v>9</v>
@@ -3187,9 +3184,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B43" t="s">
         <v>3</v>
@@ -3204,10 +3201,10 @@
         <v>8</v>
       </c>
       <c r="F43" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G43" t="s">
-        <v>44</v>
+        <v>7</v>
       </c>
       <c r="H43" t="s">
         <v>23</v>
@@ -3216,13 +3213,13 @@
         <v>9</v>
       </c>
       <c r="J43" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="K43" t="s">
-        <v>107</v>
+        <v>56</v>
       </c>
       <c r="L43" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="M43" t="s">
         <v>8</v>
@@ -3231,7 +3228,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>108</v>
       </c>
@@ -3248,13 +3245,13 @@
         <v>8</v>
       </c>
       <c r="F44" t="s">
-        <v>88</v>
+        <v>14</v>
       </c>
       <c r="G44" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="H44" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="I44" t="s">
         <v>9</v>
@@ -3263,10 +3260,10 @@
         <v>8</v>
       </c>
       <c r="K44" t="s">
-        <v>57</v>
+        <v>109</v>
       </c>
       <c r="L44" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="M44" t="s">
         <v>8</v>
@@ -3275,9 +3272,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B45" t="s">
         <v>3</v>
@@ -3292,13 +3289,13 @@
         <v>8</v>
       </c>
       <c r="F45" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="G45" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="H45" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="I45" t="s">
         <v>9</v>
@@ -3307,7 +3304,7 @@
         <v>8</v>
       </c>
       <c r="K45" t="s">
-        <v>110</v>
+        <v>38</v>
       </c>
       <c r="L45" t="s">
         <v>9</v>
@@ -3319,7 +3316,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>111</v>
       </c>
@@ -3330,28 +3327,28 @@
         <v>4</v>
       </c>
       <c r="D46" t="s">
-        <v>20</v>
+        <v>96</v>
       </c>
       <c r="E46">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F46" t="s">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="G46" t="s">
         <v>7</v>
       </c>
       <c r="H46" t="s">
-        <v>11</v>
+        <v>48</v>
       </c>
       <c r="I46" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="J46" t="s">
         <v>8</v>
       </c>
       <c r="K46" t="s">
-        <v>39</v>
+        <v>10</v>
       </c>
       <c r="L46" t="s">
         <v>9</v>
@@ -3363,7 +3360,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>112</v>
       </c>
@@ -3374,7 +3371,7 @@
         <v>4</v>
       </c>
       <c r="D47" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E47">
         <v>5</v>
@@ -3383,31 +3380,31 @@
         <v>14</v>
       </c>
       <c r="G47" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="H47" t="s">
-        <v>49</v>
+        <v>17</v>
       </c>
       <c r="I47" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="J47" t="s">
         <v>8</v>
       </c>
       <c r="K47" t="s">
-        <v>10</v>
+        <v>38</v>
       </c>
       <c r="L47" t="s">
         <v>9</v>
       </c>
       <c r="M47" t="s">
-        <v>8</v>
+        <v>37</v>
       </c>
       <c r="N47" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>113</v>
       </c>
@@ -3418,19 +3415,19 @@
         <v>4</v>
       </c>
       <c r="D48" t="s">
-        <v>97</v>
+        <v>20</v>
       </c>
       <c r="E48">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F48" t="s">
-        <v>14</v>
+        <v>53</v>
       </c>
       <c r="G48" t="s">
-        <v>44</v>
+        <v>7</v>
       </c>
       <c r="H48" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="I48" t="s">
         <v>9</v>
@@ -3439,63 +3436,63 @@
         <v>8</v>
       </c>
       <c r="K48" t="s">
-        <v>39</v>
+        <v>64</v>
       </c>
       <c r="L48" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="M48" t="s">
-        <v>38</v>
+        <v>8</v>
       </c>
       <c r="N48" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
+        <v>115</v>
+      </c>
+      <c r="B49" t="s">
+        <v>3</v>
+      </c>
+      <c r="C49" t="s">
+        <v>4</v>
+      </c>
+      <c r="D49" t="s">
+        <v>20</v>
+      </c>
+      <c r="E49">
+        <v>8</v>
+      </c>
+      <c r="F49" t="s">
+        <v>6</v>
+      </c>
+      <c r="G49" t="s">
+        <v>7</v>
+      </c>
+      <c r="H49" t="s">
+        <v>11</v>
+      </c>
+      <c r="I49" t="s">
+        <v>9</v>
+      </c>
+      <c r="J49" t="s">
+        <v>26</v>
+      </c>
+      <c r="K49" t="s">
         <v>114</v>
       </c>
-      <c r="B49" t="s">
-        <v>3</v>
-      </c>
-      <c r="C49" t="s">
-        <v>4</v>
-      </c>
-      <c r="D49" t="s">
-        <v>20</v>
-      </c>
-      <c r="E49">
-        <v>8</v>
-      </c>
-      <c r="F49" t="s">
-        <v>54</v>
-      </c>
-      <c r="G49" t="s">
-        <v>7</v>
-      </c>
-      <c r="H49" t="s">
-        <v>31</v>
-      </c>
-      <c r="I49" t="s">
-        <v>9</v>
-      </c>
-      <c r="J49" t="s">
-        <v>8</v>
-      </c>
-      <c r="K49" t="s">
-        <v>65</v>
-      </c>
       <c r="L49" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="M49" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="N49" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>116</v>
       </c>
@@ -3515,33 +3512,33 @@
         <v>6</v>
       </c>
       <c r="G50" t="s">
-        <v>7</v>
+        <v>36</v>
       </c>
       <c r="H50" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="I50" t="s">
         <v>9</v>
       </c>
       <c r="J50" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="K50" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="L50" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="M50" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="N50" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B51" t="s">
         <v>3</v>
@@ -3556,25 +3553,25 @@
         <v>8</v>
       </c>
       <c r="F51" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="G51" t="s">
-        <v>37</v>
+        <v>7</v>
       </c>
       <c r="H51" t="s">
-        <v>23</v>
+        <v>48</v>
       </c>
       <c r="I51" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="J51" t="s">
         <v>8</v>
       </c>
       <c r="K51" t="s">
-        <v>118</v>
+        <v>34</v>
       </c>
       <c r="L51" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="M51" t="s">
         <v>8</v>
@@ -3583,7 +3580,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>119</v>
       </c>
@@ -3600,36 +3597,36 @@
         <v>8</v>
       </c>
       <c r="F52" t="s">
-        <v>14</v>
+        <v>87</v>
       </c>
       <c r="G52" t="s">
         <v>7</v>
       </c>
       <c r="H52" t="s">
-        <v>49</v>
+        <v>30</v>
       </c>
       <c r="I52" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="J52" t="s">
         <v>8</v>
       </c>
       <c r="K52" t="s">
-        <v>35</v>
+        <v>120</v>
       </c>
       <c r="L52" t="s">
         <v>9</v>
       </c>
       <c r="M52" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="N52" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B53" t="s">
         <v>3</v>
@@ -3644,13 +3641,13 @@
         <v>8</v>
       </c>
       <c r="F53" t="s">
-        <v>88</v>
+        <v>28</v>
       </c>
       <c r="G53" t="s">
         <v>7</v>
       </c>
       <c r="H53" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="I53" t="s">
         <v>9</v>
@@ -3659,21 +3656,21 @@
         <v>8</v>
       </c>
       <c r="K53" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="L53" t="s">
         <v>9</v>
       </c>
       <c r="M53" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="N53" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B54" t="s">
         <v>3</v>
@@ -3682,13 +3679,13 @@
         <v>4</v>
       </c>
       <c r="D54" t="s">
-        <v>20</v>
+        <v>96</v>
       </c>
       <c r="E54">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F54" t="s">
-        <v>29</v>
+        <v>87</v>
       </c>
       <c r="G54" t="s">
         <v>7</v>
@@ -3703,7 +3700,7 @@
         <v>8</v>
       </c>
       <c r="K54" t="s">
-        <v>123</v>
+        <v>56</v>
       </c>
       <c r="L54" t="s">
         <v>9</v>
@@ -3715,7 +3712,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>124</v>
       </c>
@@ -3726,19 +3723,19 @@
         <v>4</v>
       </c>
       <c r="D55" t="s">
-        <v>97</v>
+        <v>20</v>
       </c>
       <c r="E55">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F55" t="s">
-        <v>88</v>
+        <v>53</v>
       </c>
       <c r="G55" t="s">
         <v>7</v>
       </c>
       <c r="H55" t="s">
-        <v>17</v>
+        <v>48</v>
       </c>
       <c r="I55" t="s">
         <v>9</v>
@@ -3747,7 +3744,7 @@
         <v>8</v>
       </c>
       <c r="K55" t="s">
-        <v>57</v>
+        <v>125</v>
       </c>
       <c r="L55" t="s">
         <v>9</v>
@@ -3759,9 +3756,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B56" t="s">
         <v>3</v>
@@ -3776,25 +3773,25 @@
         <v>8</v>
       </c>
       <c r="F56" t="s">
-        <v>54</v>
+        <v>14</v>
       </c>
       <c r="G56" t="s">
         <v>7</v>
       </c>
       <c r="H56" t="s">
-        <v>49</v>
+        <v>23</v>
       </c>
       <c r="I56" t="s">
         <v>9</v>
       </c>
       <c r="J56" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="K56" t="s">
-        <v>126</v>
+        <v>67</v>
       </c>
       <c r="L56" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="M56" t="s">
         <v>8</v>
@@ -3803,7 +3800,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>127</v>
       </c>
@@ -3814,10 +3811,10 @@
         <v>4</v>
       </c>
       <c r="D57" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="E57">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="F57" t="s">
         <v>14</v>
@@ -3826,19 +3823,19 @@
         <v>7</v>
       </c>
       <c r="H57" t="s">
-        <v>23</v>
+        <v>44</v>
       </c>
       <c r="I57" t="s">
         <v>9</v>
       </c>
       <c r="J57" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="K57" t="s">
-        <v>68</v>
+        <v>128</v>
       </c>
       <c r="L57" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="M57" t="s">
         <v>8</v>
@@ -3847,9 +3844,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B58" t="s">
         <v>3</v>
@@ -3858,10 +3855,10 @@
         <v>4</v>
       </c>
       <c r="D58" t="s">
+        <v>96</v>
+      </c>
+      <c r="E58">
         <v>5</v>
-      </c>
-      <c r="E58">
-        <v>2</v>
       </c>
       <c r="F58" t="s">
         <v>14</v>
@@ -3870,7 +3867,7 @@
         <v>7</v>
       </c>
       <c r="H58" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I58" t="s">
         <v>9</v>
@@ -3879,7 +3876,7 @@
         <v>8</v>
       </c>
       <c r="K58" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="L58" t="s">
         <v>9</v>
@@ -3891,7 +3888,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>130</v>
       </c>
@@ -3902,7 +3899,7 @@
         <v>4</v>
       </c>
       <c r="D59" t="s">
-        <v>97</v>
+        <v>20</v>
       </c>
       <c r="E59">
         <v>5</v>
@@ -3914,7 +3911,7 @@
         <v>7</v>
       </c>
       <c r="H59" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I59" t="s">
         <v>9</v>
@@ -3923,7 +3920,7 @@
         <v>8</v>
       </c>
       <c r="K59" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="L59" t="s">
         <v>9</v>
@@ -3935,7 +3932,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>131</v>
       </c>
@@ -3949,7 +3946,7 @@
         <v>20</v>
       </c>
       <c r="E60">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F60" t="s">
         <v>14</v>
@@ -3958,7 +3955,7 @@
         <v>7</v>
       </c>
       <c r="H60" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="I60" t="s">
         <v>9</v>
@@ -3967,19 +3964,19 @@
         <v>8</v>
       </c>
       <c r="K60" t="s">
-        <v>129</v>
+        <v>38</v>
       </c>
       <c r="L60" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="M60" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="N60" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>132</v>
       </c>
@@ -3996,10 +3993,10 @@
         <v>8</v>
       </c>
       <c r="F61" t="s">
-        <v>14</v>
+        <v>53</v>
       </c>
       <c r="G61" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="H61" t="s">
         <v>17</v>
@@ -4011,19 +4008,19 @@
         <v>8</v>
       </c>
       <c r="K61" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="L61" t="s">
         <v>15</v>
       </c>
       <c r="M61" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="N61" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>133</v>
       </c>
@@ -4034,20 +4031,20 @@
         <v>4</v>
       </c>
       <c r="D62" t="s">
-        <v>20</v>
+        <v>96</v>
       </c>
       <c r="E62">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F62" t="s">
-        <v>54</v>
+        <v>14</v>
       </c>
       <c r="G62" t="s">
+        <v>7</v>
+      </c>
+      <c r="H62" t="s">
         <v>44</v>
       </c>
-      <c r="H62" t="s">
-        <v>17</v>
-      </c>
       <c r="I62" t="s">
         <v>9</v>
       </c>
@@ -4055,7 +4052,7 @@
         <v>8</v>
       </c>
       <c r="K62" t="s">
-        <v>33</v>
+        <v>128</v>
       </c>
       <c r="L62" t="s">
         <v>15</v>
@@ -4067,7 +4064,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>134</v>
       </c>
@@ -4078,10 +4075,10 @@
         <v>4</v>
       </c>
       <c r="D63" t="s">
-        <v>97</v>
+        <v>5</v>
       </c>
       <c r="E63">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F63" t="s">
         <v>14</v>
@@ -4090,7 +4087,7 @@
         <v>7</v>
       </c>
       <c r="H63" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="I63" t="s">
         <v>9</v>
@@ -4099,10 +4096,10 @@
         <v>8</v>
       </c>
       <c r="K63" t="s">
-        <v>129</v>
+        <v>56</v>
       </c>
       <c r="L63" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="M63" t="s">
         <v>8</v>
@@ -4111,7 +4108,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>135</v>
       </c>
@@ -4134,7 +4131,7 @@
         <v>7</v>
       </c>
       <c r="H64" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="I64" t="s">
         <v>9</v>
@@ -4143,10 +4140,10 @@
         <v>8</v>
       </c>
       <c r="K64" t="s">
-        <v>57</v>
+        <v>128</v>
       </c>
       <c r="L64" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="M64" t="s">
         <v>8</v>
@@ -4155,7 +4152,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>136</v>
       </c>
@@ -4178,16 +4175,16 @@
         <v>7</v>
       </c>
       <c r="H65" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I65" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="J65" t="s">
         <v>8</v>
       </c>
       <c r="K65" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="L65" t="s">
         <v>15</v>
@@ -4199,7 +4196,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>137</v>
       </c>
@@ -4210,10 +4207,10 @@
         <v>4</v>
       </c>
       <c r="D66" t="s">
+        <v>96</v>
+      </c>
+      <c r="E66">
         <v>5</v>
-      </c>
-      <c r="E66">
-        <v>2</v>
       </c>
       <c r="F66" t="s">
         <v>14</v>
@@ -4222,7 +4219,7 @@
         <v>7</v>
       </c>
       <c r="H66" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I66" t="s">
         <v>15</v>
@@ -4231,7 +4228,7 @@
         <v>8</v>
       </c>
       <c r="K66" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="L66" t="s">
         <v>15</v>
@@ -4243,7 +4240,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>138</v>
       </c>
@@ -4254,42 +4251,42 @@
         <v>4</v>
       </c>
       <c r="D67" t="s">
-        <v>97</v>
+        <v>20</v>
       </c>
       <c r="E67">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F67" t="s">
         <v>14</v>
       </c>
       <c r="G67" t="s">
-        <v>7</v>
+        <v>36</v>
       </c>
       <c r="H67" t="s">
-        <v>45</v>
+        <v>139</v>
       </c>
       <c r="I67" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="J67" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="K67" t="s">
-        <v>129</v>
+        <v>10</v>
       </c>
       <c r="L67" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="M67" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="N67" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B68" t="s">
         <v>3</v>
@@ -4304,36 +4301,36 @@
         <v>8</v>
       </c>
       <c r="F68" t="s">
-        <v>14</v>
+        <v>87</v>
       </c>
       <c r="G68" t="s">
-        <v>37</v>
+        <v>7</v>
       </c>
       <c r="H68" t="s">
-        <v>140</v>
+        <v>23</v>
       </c>
       <c r="I68" t="s">
         <v>9</v>
       </c>
       <c r="J68" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="K68" t="s">
-        <v>10</v>
+        <v>141</v>
       </c>
       <c r="L68" t="s">
         <v>9</v>
       </c>
       <c r="M68" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="N68" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B69" t="s">
         <v>3</v>
@@ -4348,10 +4345,10 @@
         <v>8</v>
       </c>
       <c r="F69" t="s">
-        <v>88</v>
+        <v>53</v>
       </c>
       <c r="G69" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="H69" t="s">
         <v>23</v>
@@ -4363,10 +4360,10 @@
         <v>8</v>
       </c>
       <c r="K69" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="L69" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="M69" t="s">
         <v>8</v>
@@ -4375,9 +4372,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B70" t="s">
         <v>3</v>
@@ -4392,81 +4389,37 @@
         <v>8</v>
       </c>
       <c r="F70" t="s">
-        <v>54</v>
+        <v>14</v>
       </c>
       <c r="G70" t="s">
-        <v>44</v>
+        <v>7</v>
       </c>
       <c r="H70" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="I70" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="J70" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="K70" t="s">
-        <v>144</v>
+        <v>10</v>
       </c>
       <c r="L70" t="s">
         <v>15</v>
       </c>
       <c r="M70" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="N70" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A71" t="s">
-        <v>145</v>
-      </c>
-      <c r="B71" t="s">
-        <v>3</v>
-      </c>
-      <c r="C71" t="s">
-        <v>4</v>
-      </c>
-      <c r="D71" t="s">
-        <v>20</v>
-      </c>
-      <c r="E71">
-        <v>8</v>
-      </c>
-      <c r="F71" t="s">
-        <v>14</v>
-      </c>
-      <c r="G71" t="s">
-        <v>7</v>
-      </c>
-      <c r="H71" t="s">
-        <v>17</v>
-      </c>
-      <c r="I71" t="s">
-        <v>15</v>
-      </c>
-      <c r="J71" t="s">
-        <v>25</v>
-      </c>
-      <c r="K71" t="s">
-        <v>10</v>
-      </c>
-      <c r="L71" t="s">
-        <v>15</v>
-      </c>
-      <c r="M71" t="s">
-        <v>25</v>
-      </c>
-      <c r="N71" t="s">
-        <v>13</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:P30" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:U32">
-    <sortCondition ref="A2:A32"/>
+  <autoFilter ref="A1:P29" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:U31">
+    <sortCondition ref="A2:A31"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>